<commit_message>
fixedFiles added passing tests
</commit_message>
<xml_diff>
--- a/Clue2/board.xlsx
+++ b/Clue2/board.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="18">
   <si>
     <t>W</t>
   </si>
@@ -27,9 +27,6 @@
     <t>3L</t>
   </si>
   <si>
-    <t>1R</t>
-  </si>
-  <si>
     <t>2D</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>git</t>
+  </si>
+  <si>
+    <t>1D</t>
   </si>
 </sst>
 </file>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.88671875" defaultRowHeight="14.4"/>
@@ -635,12 +635,12 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K4" s="3">
         <v>2</v>
@@ -681,7 +681,7 @@
         <v>3</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S4" s="3">
         <v>3</v>
@@ -831,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3">
         <v>4</v>
@@ -851,11 +851,11 @@
       <c r="I7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>0</v>
+      <c r="J7" s="3">
+        <v>9</v>
+      </c>
+      <c r="K7" s="3">
+        <v>9</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>5</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S7" s="3">
         <v>5</v>
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O8" s="3">
         <v>5</v>
@@ -973,7 +973,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>0</v>
@@ -985,7 +985,7 @@
         <v>9</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>0</v>
@@ -1136,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S11" s="3">
         <v>5</v>
@@ -1227,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="3">
         <v>6</v>
@@ -1248,7 +1248,7 @@
         <v>7</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M13" s="3">
         <v>7</v>
@@ -1266,7 +1266,7 @@
         <v>8</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S13" s="3">
         <v>8</v>
@@ -1301,7 +1301,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>0</v>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q14" s="3">
         <v>8</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="22" spans="8:8">
       <c r="H22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>